<commit_message>
update and delete api's
</commit_message>
<xml_diff>
--- a/blogs_api.xlsx
+++ b/blogs_api.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WEBSITES\Django Backends\blog_app_backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B86A00B-2188-472A-9A46-104FE9FE8A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18262F39-B568-4C11-BB21-86D989D57563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>API name</t>
   </si>
@@ -129,6 +129,48 @@
   </si>
   <si>
     <t>{"id":"1"}</t>
+  </si>
+  <si>
+    <t>Update Blog</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/api/updateMy/</t>
+  </si>
+  <si>
+    <t>{"userid": "18","id":"1" "title": "Asim's blog", "post": "ambalavaasi"}</t>
+  </si>
+  <si>
+    <t>{"status":"post updated"}</t>
+  </si>
+  <si>
+    <t>{"status":"post Deleted"}</t>
+  </si>
+  <si>
+    <t>{"title":"Asim's blog"}</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/api/deleteMy/</t>
+  </si>
+  <si>
+    <t>Delete Blog</t>
+  </si>
+  <si>
+    <t>Display Update</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/api/displayUpdateMy/</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>{"userid":"1", "id":"9"}</t>
+  </si>
+  <si>
+    <t>[{"id": 9, "userid": 1, "title": "test", "post": "test"}]</t>
   </si>
 </sst>
 </file>
@@ -181,7 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -195,9 +237,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -480,16 +521,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="33.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="44.6640625" style="2" customWidth="1"/>
@@ -553,7 +594,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -569,11 +610,14 @@
         <v>17</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+    </row>
     <row r="9" spans="1:6" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -583,11 +627,14 @@
         <v>21</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+    </row>
     <row r="11" spans="1:6" ht="151.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -600,11 +647,14 @@
         <v>24</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+    </row>
     <row r="13" spans="1:6" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -614,11 +664,14 @@
         <v>27</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+    </row>
     <row r="15" spans="1:6" ht="152.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -632,7 +685,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -646,6 +699,60 @@
       </c>
       <c r="E16" s="4" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" ht="159" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="173.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="129" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -658,8 +765,11 @@
     <hyperlink ref="B13" r:id="rId6" xr:uid="{80A6FEAA-3580-4028-814E-7751EB78587D}"/>
     <hyperlink ref="B15" r:id="rId7" xr:uid="{19D35537-2B99-418A-9196-887C12AD3A9E}"/>
     <hyperlink ref="B16" r:id="rId8" xr:uid="{2EE45D5E-6005-473C-ADC7-F05FC2EE45AE}"/>
+    <hyperlink ref="B18" r:id="rId9" xr:uid="{31816004-66ED-4EB1-9AC8-9B0055F0C9E5}"/>
+    <hyperlink ref="B20" r:id="rId10" xr:uid="{014C6A27-A46A-46D0-B7B4-80AFB8A07C00}"/>
+    <hyperlink ref="B22" r:id="rId11" xr:uid="{D71EC552-DE9D-4F72-A142-4832A7A9733D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>